<commit_message>
(feat) RDCC-2261 : Adding S2S functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/ServiceRoleMapping_BBA9.xlsx
+++ b/src/test/resources/ServiceRoleMapping_BBA9.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:8001_{636E706E-9221-2E46-920A-CC7DDC75B439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F245E94-5576-F447-89EA-50B6CCAB5A54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>